<commit_message>
Added Ticket to Ride: Pennsylvania files
</commit_message>
<xml_diff>
--- a/Europe_Data_Files/Europe_Routes.xlsx
+++ b/Europe_Data_Files/Europe_Routes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a684b2255d33441d/Data_science_projects/Ticket_To_Ride/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a684b2255d33441d/Data_science_projects/Ticket_To_Ride/Europe_Data_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1170" documentId="19281AB09AA5727DDAE0A0A58762F9AD941FED7A" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{B357A796-E18B-4780-9146-75EAB154F323}"/>
+  <xr:revisionPtr revIDLastSave="1172" documentId="19281AB09AA5727DDAE0A0A58762F9AD941FED7A" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{888B7101-CA09-4E80-ABEC-F91165026B90}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{FA475A58-E653-40FB-A462-05AA0B81D925}"/>
   </bookViews>
@@ -3637,7 +3637,7 @@
   <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>